<commit_message>
map generation rework started
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Terrains.xlsx
+++ b/OpenWorld/Resources/Terrains.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248174A9-F7DF-4977-ABC7-BD15E35A0AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -110,12 +111,15 @@
   </si>
   <si>
     <t>Light forest</t>
+  </si>
+  <si>
+    <t>Fox,Wolf,Wild boar,Fairy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -165,7 +169,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -240,6 +244,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -275,6 +296,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -450,11 +488,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +631,12 @@
       <c r="A11" t="s">
         <v>31</v>
       </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
kinda working, requirement check added, but doublke cave from one mountain should be eleminated
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Terrains.xlsx
+++ b/OpenWorld/Resources/Terrains.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248174A9-F7DF-4977-ABC7-BD15E35A0AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -15,29 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
-  <si>
-    <t xml:space="preserve">name </t>
-  </si>
-  <si>
-    <t>Meadow</t>
-  </si>
-  <si>
-    <t>Mountain</t>
-  </si>
-  <si>
-    <t>Riverside</t>
-  </si>
-  <si>
-    <t>Road</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Fox,Wolf</t>
   </si>
   <si>
-    <t>Lake</t>
-  </si>
-  <si>
     <t>Mermaid,Fairy</t>
   </si>
   <si>
@@ -47,18 +28,12 @@
     <t>Fox,Fairy</t>
   </si>
   <si>
-    <t>Cave in the forest</t>
-  </si>
-  <si>
     <t>Cave troll,Werewolf,Ghost,Zombie,Orc,Goblin</t>
   </si>
   <si>
     <t>Fox,Wolf,Wild boar,Werewolf,Fairy</t>
   </si>
   <si>
-    <t>Cave in the mountains</t>
-  </si>
-  <si>
     <t>Cave troll,Werewolf,Dragon,Stone golem</t>
   </si>
   <si>
@@ -86,40 +61,58 @@
     <t>Fox,Mermaid</t>
   </si>
   <si>
-    <t>Fox</t>
-  </si>
-  <si>
     <t>Mermaid</t>
   </si>
   <si>
     <t>Cave troll,Dragon,Stone golem</t>
   </si>
   <si>
-    <t>previousPath</t>
-  </si>
-  <si>
-    <t>Bridge</t>
-  </si>
-  <si>
     <t>Mermaid,Troll</t>
   </si>
   <si>
     <t>Mermaid,Fairy,Troll</t>
   </si>
   <si>
-    <t>Deep forest</t>
-  </si>
-  <si>
-    <t>Light forest</t>
-  </si>
-  <si>
     <t>Fox,Wolf,Wild boar,Fairy</t>
+  </si>
+  <si>
+    <t>travelName</t>
+  </si>
+  <si>
+    <t>Deeper into the forest</t>
+  </si>
+  <si>
+    <t>To the mountains</t>
+  </si>
+  <si>
+    <t>Into a cave in this forest</t>
+  </si>
+  <si>
+    <t>In the direction of light forest</t>
+  </si>
+  <si>
+    <t>To a lake</t>
+  </si>
+  <si>
+    <t>Follow a stream nearby</t>
+  </si>
+  <si>
+    <t>To a meadow nearby</t>
+  </si>
+  <si>
+    <t>Cross this bridge</t>
+  </si>
+  <si>
+    <t>previousTerrain</t>
+  </si>
+  <si>
+    <t>Into a cave on this mountain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -169,7 +162,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -244,23 +237,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -296,23 +272,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -488,154 +447,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
+      <c r="D8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
map generation works, needs requs
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Terrains.xlsx
+++ b/OpenWorld/Resources/Terrains.xlsx
@@ -100,9 +100,6 @@
     <t>To a meadow nearby</t>
   </si>
   <si>
-    <t>Cross this bridge</t>
-  </si>
-  <si>
     <t>Into a cave on this mountain</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>numOfEntrances</t>
+  </si>
+  <si>
+    <t>Cross a bridge</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,16 +508,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -528,13 +528,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -545,7 +545,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -573,13 +573,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -621,13 +621,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -641,13 +641,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -672,19 +672,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
traveling with requs is working, ugly solution added
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Terrains.xlsx
+++ b/OpenWorld/Resources/Terrains.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>Fox,Wolf</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Wolf,Wild boar,Stone golem,Giant</t>
   </si>
   <si>
-    <t>enemiesDay</t>
-  </si>
-  <si>
-    <t>enemiesNight</t>
-  </si>
-  <si>
     <t>Fox,Wolf,Wild boar</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>Fox,Wolf,Wild boar,Fairy</t>
   </si>
   <si>
-    <t>travelName</t>
-  </si>
-  <si>
     <t>Deeper into the forest</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>Into a cave on this mountain</t>
   </si>
   <si>
-    <t>placeName</t>
-  </si>
-  <si>
     <t>Deep into the forest</t>
   </si>
   <si>
@@ -142,15 +130,9 @@
     <t>Wild boar</t>
   </si>
   <si>
-    <t>requiredPreviousTerrain</t>
-  </si>
-  <si>
     <t>Cross a bridge</t>
   </si>
   <si>
-    <t>fixedConnectionSize</t>
-  </si>
-  <si>
     <t>Bandit,Wolf</t>
   </si>
   <si>
@@ -175,9 +157,6 @@
     <t>Onto a tundra</t>
   </si>
   <si>
-    <t>On frozen land</t>
-  </si>
-  <si>
     <t>Towards snowy slopes</t>
   </si>
   <si>
@@ -200,6 +179,36 @@
   </si>
   <si>
     <t>Towards wet barren land</t>
+  </si>
+  <si>
+    <t>Enemies during the day</t>
+  </si>
+  <si>
+    <t>Enemies during the night</t>
+  </si>
+  <si>
+    <t>Name of the place</t>
+  </si>
+  <si>
+    <t>Name of travel option to get there</t>
+  </si>
+  <si>
+    <t>Required previous place name</t>
+  </si>
+  <si>
+    <t>Required following place names</t>
+  </si>
+  <si>
+    <t>On a frozen snowland</t>
+  </si>
+  <si>
+    <t>Deep into the forest;At the other exit of the cave</t>
+  </si>
+  <si>
+    <t>In the mountains;At the other exit of the cave</t>
+  </si>
+  <si>
+    <t>On wet, barren soil;On a frozen snowland;In a lightly forested area;On the side of a stream;On the shore of a lake;On frozen land;On the shore of a river;On the shores of an ocean;Swamp</t>
   </si>
 </sst>
 </file>
@@ -544,7 +553,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,43 +561,43 @@
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="170.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -596,47 +605,47 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -644,13 +653,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
@@ -658,13 +667,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
@@ -672,19 +681,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+      <c r="D8" t="s">
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -692,195 +701,186 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Map generation tweaked a bit, 2 destination max without a map
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Terrains.xlsx
+++ b/OpenWorld/Resources/Terrains.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B4E6CD-2550-4E4E-9953-ED25BD5A1315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>Fox,Wolf</t>
   </si>
@@ -142,15 +143,6 @@
     <t>Into a desert</t>
   </si>
   <si>
-    <t>Towards dry barren land</t>
-  </si>
-  <si>
-    <t>On dry, barren soil</t>
-  </si>
-  <si>
-    <t>On wet, barren soil</t>
-  </si>
-  <si>
     <t>On a tundra</t>
   </si>
   <si>
@@ -178,9 +170,6 @@
     <t>Into a swamp</t>
   </si>
   <si>
-    <t>Towards wet barren land</t>
-  </si>
-  <si>
     <t>Enemies during the day</t>
   </si>
   <si>
@@ -208,13 +197,25 @@
     <t>In the mountains;At the other exit of the cave</t>
   </si>
   <si>
-    <t>On wet, barren soil;On a frozen snowland;In a lightly forested area;On the side of a stream;On the shore of a lake;On frozen land;On the shore of a river;On the shores of an ocean;Swamp</t>
+    <t>On dry ground</t>
+  </si>
+  <si>
+    <t>On wet ground</t>
+  </si>
+  <si>
+    <t>Towards wet land</t>
+  </si>
+  <si>
+    <t>Towards dry land</t>
+  </si>
+  <si>
+    <t>On wet ground;On a frozen snowland;In a lightly forested area;On the side of a stream;On the shore of a lake;On frozen land;On the shore of a river;On the shores of an ocean;Swamp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -264,7 +265,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -339,6 +340,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -374,6 +392,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -549,11 +584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,22 +603,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -642,7 +677,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -690,7 +725,7 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -749,10 +784,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
@@ -769,10 +804,10 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
@@ -783,10 +818,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
         <v>39</v>
@@ -797,13 +832,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
         <v>64</v>
@@ -817,16 +852,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
         <v>39</v>
@@ -837,10 +872,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
@@ -854,13 +889,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
         <v>39</v>
@@ -871,10 +906,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
       </c>
       <c r="E19" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
bfs search for path works with map
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Terrains.xlsx
+++ b/OpenWorld/Resources/Terrains.xlsx
@@ -163,9 +163,6 @@
     <t>On the shores of an ocean</t>
   </si>
   <si>
-    <t>Swamp</t>
-  </si>
-  <si>
     <t>Into a swamp</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>Enemies during the night</t>
   </si>
   <si>
-    <t>Name of the place</t>
-  </si>
-  <si>
     <t>Name of travel option to get there</t>
   </si>
   <si>
@@ -209,6 +203,12 @@
   </si>
   <si>
     <t>On wet ground;On a frozen snowland;In a lightly forested area;On the side of a stream;On the shore of a lake;On frozen land;On the shore of a river;On the shores of an ocean;Swamp</t>
+  </si>
+  <si>
+    <t>In a swamp</t>
+  </si>
+  <si>
+    <t>Name of place when there</t>
   </si>
 </sst>
 </file>
@@ -563,12 +563,12 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="170.140625" bestFit="1" customWidth="1"/>
@@ -578,22 +578,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -700,7 +700,7 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -759,10 +759,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
@@ -779,10 +779,10 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
@@ -793,10 +793,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
         <v>39</v>
@@ -813,10 +813,10 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>39</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
terrains populated with enemies
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Terrains.xlsx
+++ b/OpenWorld/Resources/Terrains.xlsx
@@ -14,61 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
-  <si>
-    <t>Fox,Wolf</t>
-  </si>
-  <si>
-    <t>Mermaid,Fairy</t>
-  </si>
-  <si>
-    <t>Fox,Fairy,Mermaid</t>
-  </si>
-  <si>
-    <t>Fox,Fairy</t>
-  </si>
-  <si>
-    <t>Cave troll,Werewolf,Ghost,Zombie,Orc,Goblin</t>
-  </si>
-  <si>
-    <t>Fox,Wolf,Wild boar,Werewolf,Fairy</t>
-  </si>
-  <si>
-    <t>Cave troll,Werewolf,Dragon,Stone golem</t>
-  </si>
-  <si>
-    <t>Wolf,Wild boar,Stone golem,Giant</t>
-  </si>
-  <si>
-    <t>Fox,Wolf,Wild boar</t>
-  </si>
-  <si>
-    <t>Fox,Fairy,Wolf,Wild boar</t>
-  </si>
-  <si>
-    <t>Wolf,Wild boar,Stone golem,Giant,Orc,Goblin</t>
-  </si>
-  <si>
-    <t>Cave troll,Zombie,Orc,Goblin</t>
-  </si>
-  <si>
-    <t>Fox,Mermaid</t>
-  </si>
-  <si>
-    <t>Mermaid</t>
-  </si>
-  <si>
-    <t>Cave troll,Dragon,Stone golem</t>
-  </si>
-  <si>
-    <t>Mermaid,Troll</t>
-  </si>
-  <si>
-    <t>Mermaid,Fairy,Troll</t>
-  </si>
-  <si>
-    <t>Fox,Wolf,Wild boar,Fairy</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>Deeper into the forest</t>
   </si>
@@ -124,18 +70,9 @@
     <t>At the other exit of the cave</t>
   </si>
   <si>
-    <t>Bandit,Troll</t>
-  </si>
-  <si>
-    <t>Wild boar</t>
-  </si>
-  <si>
     <t>Cross a bridge</t>
   </si>
   <si>
-    <t>Bandit,Wolf</t>
-  </si>
-  <si>
     <t>In a desert</t>
   </si>
   <si>
@@ -209,6 +146,114 @@
   </si>
   <si>
     <t>Name of place when there</t>
+  </si>
+  <si>
+    <t>Bandit,Troll,Cannibal</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Cannibal</t>
+  </si>
+  <si>
+    <t>Mermaid,Troll,Cannibal</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Cannibal,Infernal Fiend,Manticore</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Basilisk,Manticore</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Cannibal,Infernal Fiend,Mad Knight,Shadow Demon</t>
+  </si>
+  <si>
+    <t>Mermaid,Fairy,Troll,Cannibal,Mad Knight,Shadow Demon</t>
+  </si>
+  <si>
+    <t>Wolf,Wild boar,Stone golem,Giant,Orc,Goblin,Dragon,Gargoyle,Shadow Demon,Skeleton</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Cannibal,Mad Knight,Naga,Shadow Demon,Specter</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Dragon,Hag,Naga,Shadow Demon,Specter</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Naga,Sea Serpent,The Krakken</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Mad Knight,Sea Serpent,Shadow Demon,The Krakken</t>
+  </si>
+  <si>
+    <t>Fox,Wolf,Wild boar,Cannibal,Carnivorous Plant,Centaur,Ent,Fungoid,Kobold,Toxic Spore</t>
+  </si>
+  <si>
+    <t>Fox,Wolf,Wild boar,Werewolf,Fairy,Acromantula,Cannibal,Carnivorous Plant,Centaur,Ent,Fungoid,Hag,Kobold,Shadow Demon,Specter,Toxic Spore</t>
+  </si>
+  <si>
+    <t>Fox,Mermaid,Griffon,Toxic Spore</t>
+  </si>
+  <si>
+    <t>Fox,Fairy,Mermaid,Fungoid,Kobold,Manticore,Shadow Demon,Toxic Spore</t>
+  </si>
+  <si>
+    <t>Mermaid,Griffon,Sea Serpent,The Krakken,Toxic Spore</t>
+  </si>
+  <si>
+    <t>Mermaid,Fairy,Fungoid,Ent,Gargoyle,Hag,Mad Knight,Naga,Sea Serpent,Shadow Demon,The Krakken,Toxic Spore</t>
+  </si>
+  <si>
+    <t>Cave troll,Zombie,Orc,Goblin,Acromantula,Basilisk,Cannibal,Dragon,Gargoyle,Skeleton,Vampire</t>
+  </si>
+  <si>
+    <t>Cave troll,Dragon,Stone golem,Acromantula,Basilisk,Cannibal,Dragon,Manticore,Skeleton,Vampire</t>
+  </si>
+  <si>
+    <t>Fox,Wolf,Wild boar,Fairy,Cannibal,Carnivorous Plant,Centaur,Ent,Fungoid,Kobold,Mad Knight,Shadow Demon,Succubus,Toxic Spore,Vampire</t>
+  </si>
+  <si>
+    <t>Fox,Fairy,Wolf,Wild boar,Griffon,Kobold,Shadow Demon,Specter,Toxic Spore,Vampire</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Basilisk,Gargoyle,Manticore,Shadow Demon,Specter,Succubus,Vampire</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Carnivorous Plant,Fungoid,Shadow Demon,Specter,Succubus,Toxic Spore,Vampire</t>
+  </si>
+  <si>
+    <t>Cave troll,Werewolf,Dragon,Stone golem,Acromantula,Basilisk,Cannibal,Dragon,Manticore,Skeleton,Specter,Wyvern</t>
+  </si>
+  <si>
+    <t>Cave troll,Werewolf,Ghost,Zombie,Orc,Goblin,Acromantula,Basilisk,Cannibal,Dragon,Gargoyle,Skeleton,Specter,Wyvern</t>
+  </si>
+  <si>
+    <t>Wolf,Wild boar,Stone golem,Giant,Dragon,Gargoyle,Manticore,Wyvern</t>
+  </si>
+  <si>
+    <t>Fox,Wolf,Cannibal,Carnivorous Plant,Kobold,Toxic Spore,Wyvern</t>
+  </si>
+  <si>
+    <t>Fox,Fairy,Griffon,Manticore,Toxic Spore,Wyvern</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Naga,Wyvern</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Carnivorous Plant,Fungoid,Succubus,Toxic Spore,Wyvern</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Fungoid,Ent,Hag,Shadow Demon,Mermaid</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Griffon,Mermaid</t>
+  </si>
+  <si>
+    <t>Wild boar,Cannibal,Fungoid,Bandit,Mad Knight,Shadow Demon,Skeleton,Specter,Vampire,Zombie</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Acromantula,Fungoid,Hag,Shadow Demon,Skeleton,Specter,Toxic Spore,Zombie</t>
+  </si>
+  <si>
+    <t>Bandit,Wolf,Hag,Kobold,Toxic Spore,Zombie</t>
   </si>
 </sst>
 </file>
@@ -563,340 +608,343 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="170.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
       </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F19">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>